<commit_message>
Veritabanı yedeği - 25.02.2025 17:37:00
</commit_message>
<xml_diff>
--- a/tools/import/AKTARILANLAR/BOYA.xlsx
+++ b/tools/import/AKTARILANLAR/BOYA.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="18">
   <si>
     <t xml:space="preserve">Stok Kodu   </t>
   </si>
@@ -73,12 +73,6 @@
   </si>
   <si>
     <t>RAL 9005-D.SIYAH SPREY BOYA 400ML</t>
-  </si>
-  <si>
-    <t>150.05.0517.00245</t>
-  </si>
-  <si>
-    <t>GEKA CAPAK ONLEYICI KAYNAK SPREYI</t>
   </si>
 </sst>
 </file>
@@ -453,10 +447,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="M7" sqref="M7"/>
+      <selection activeCell="B4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -578,41 +572,6 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" s="2" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0</v>
-      </c>
-      <c r="K4" s="5">
-        <v>0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>